<commit_message>
add numbers for search strings + update scatterplots
</commit_message>
<xml_diff>
--- a/02 detailed reviewing results.xlsx
+++ b/02 detailed reviewing results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{25F2DF63-6672-41EB-B160-798C7BD23B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BE0E2733-190D-4817-B90C-4FE281582992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviewing Results" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1559" uniqueCount="410">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1562" uniqueCount="412">
   <si>
     <t>Title</t>
   </si>
@@ -1268,6 +1268,12 @@
   </si>
   <si>
     <t>Towards Generating Model-Driven Speech Interfaces for Digital Twins</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Found through Snowballing?</t>
   </si>
 </sst>
 </file>
@@ -2193,26 +2199,26 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="50.26171875" customWidth="1"/>
+    <col min="2" max="2" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.15625" customWidth="1"/>
+    <col min="4" max="4" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.68359375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2243,8 +2249,11 @@
       <c r="J1" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
         <v>83</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
@@ -2298,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
         <v>37</v>
       </c>
@@ -2324,7 +2333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
         <v>49</v>
       </c>
@@ -2379,7 +2388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
         <v>78</v>
       </c>
@@ -2461,7 +2470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2489,7 +2498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>88</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2560,7 +2569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
@@ -2609,7 +2618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
         <v>66</v>
       </c>
@@ -2663,8 +2672,11 @@
       <c r="J17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -2687,7 +2699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
         <v>75</v>
       </c>
@@ -2713,7 +2725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -2739,7 +2751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -2765,7 +2777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -2785,7 +2797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -2837,7 +2849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>79</v>
       </c>
@@ -2863,7 +2875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
         <v>72</v>
       </c>
@@ -2889,7 +2901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
@@ -2915,7 +2927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
         <v>11</v>
       </c>
@@ -2941,7 +2953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2967,7 +2979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
         <v>1</v>
       </c>
@@ -2995,7 +3007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
@@ -3021,7 +3033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
         <v>22</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
         <v>52</v>
       </c>
@@ -3075,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="10" t="s">
         <v>45</v>
       </c>
@@ -3101,7 +3113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
         <v>99</v>
       </c>
@@ -3127,7 +3139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10" t="s">
         <v>64</v>
       </c>
@@ -3153,7 +3165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
         <v>101</v>
       </c>
@@ -3179,7 +3191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
         <v>17</v>
       </c>
@@ -3235,7 +3247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10" t="s">
         <v>57</v>
       </c>
@@ -3265,7 +3277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="10" t="s">
         <v>7</v>
       </c>
@@ -3291,7 +3303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
         <v>21</v>
       </c>
@@ -3343,7 +3355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="10" t="s">
         <v>62</v>
       </c>
@@ -3369,7 +3381,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="10" t="s">
         <v>103</v>
       </c>
@@ -3395,7 +3407,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="10" t="s">
         <v>50</v>
       </c>
@@ -3421,7 +3433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -3450,7 +3462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="10" t="s">
         <v>71</v>
       </c>
@@ -3476,7 +3488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2" t="s">
         <v>70</v>
       </c>
@@ -3501,8 +3513,11 @@
       <c r="J49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="K49" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
         <v>39</v>
       </c>
@@ -3528,7 +3543,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10" t="s">
         <v>12</v>
       </c>
@@ -3551,7 +3566,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="10" t="s">
         <v>82</v>
       </c>
@@ -3574,7 +3589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -3594,7 +3609,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -3614,7 +3629,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>355</v>
       </c>
@@ -3636,7 +3651,7 @@
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
@@ -3656,7 +3671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>356</v>
       </c>
@@ -3678,7 +3693,7 @@
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
         <v>357</v>
       </c>
@@ -3700,7 +3715,7 @@
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
@@ -3722,7 +3737,7 @@
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2" t="s">
         <v>359</v>
       </c>
@@ -3744,7 +3759,7 @@
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2" t="s">
         <v>361</v>
       </c>
@@ -3766,7 +3781,7 @@
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="10" t="s">
         <v>84</v>
       </c>
@@ -3789,7 +3804,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2" t="s">
         <v>47</v>
       </c>
@@ -3806,7 +3821,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -3823,7 +3838,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2" t="s">
         <v>362</v>
       </c>
@@ -3845,7 +3860,7 @@
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2" t="s">
         <v>364</v>
       </c>
@@ -3867,7 +3882,7 @@
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="10" t="s">
         <v>59</v>
       </c>
@@ -3891,7 +3906,7 @@
       </c>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2" t="s">
         <v>365</v>
       </c>
@@ -3913,7 +3928,7 @@
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>85</v>
       </c>
@@ -3932,7 +3947,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>42</v>
       </c>
@@ -3949,7 +3964,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
         <v>366</v>
       </c>
@@ -3971,7 +3986,7 @@
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2" t="s">
         <v>43</v>
       </c>
@@ -3988,7 +4003,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
         <v>367</v>
       </c>
@@ -4010,7 +4025,7 @@
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2" t="s">
         <v>86</v>
       </c>
@@ -4033,7 +4048,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2" t="s">
         <v>368</v>
       </c>
@@ -4055,7 +4070,7 @@
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="10" t="s">
         <v>25</v>
       </c>
@@ -4076,7 +4091,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="10" t="s">
         <v>76</v>
       </c>
@@ -4097,7 +4112,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2" t="s">
         <v>369</v>
       </c>
@@ -4119,7 +4134,7 @@
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2" t="s">
         <v>87</v>
       </c>
@@ -4144,7 +4159,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2" t="s">
         <v>370</v>
       </c>
@@ -4162,7 +4177,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2" t="s">
         <v>371</v>
       </c>
@@ -4180,7 +4195,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="10" t="s">
         <v>77</v>
       </c>
@@ -4203,7 +4218,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2" t="s">
         <v>32</v>
       </c>
@@ -4228,7 +4243,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="10" t="s">
         <v>89</v>
       </c>
@@ -4253,7 +4268,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="10" t="s">
         <v>90</v>
       </c>
@@ -4278,7 +4293,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2" t="s">
         <v>35</v>
       </c>
@@ -4301,7 +4316,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2" t="s">
         <v>372</v>
       </c>
@@ -4319,7 +4334,7 @@
       </c>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2" t="s">
         <v>92</v>
       </c>
@@ -4344,7 +4359,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2" t="s">
         <v>373</v>
       </c>
@@ -4362,7 +4377,7 @@
       </c>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="10" t="s">
         <v>93</v>
       </c>
@@ -4385,7 +4400,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2" t="s">
         <v>14</v>
       </c>
@@ -4410,7 +4425,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="10" t="s">
         <v>58</v>
       </c>
@@ -4433,7 +4448,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2" t="s">
         <v>375</v>
       </c>
@@ -4451,7 +4466,7 @@
       </c>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2" t="s">
         <v>376</v>
       </c>
@@ -4469,7 +4484,7 @@
       </c>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2" t="s">
         <v>377</v>
       </c>
@@ -4487,7 +4502,7 @@
       </c>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2" t="s">
         <v>378</v>
       </c>
@@ -4505,7 +4520,7 @@
       </c>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2" t="s">
         <v>31</v>
       </c>
@@ -4530,7 +4545,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2" t="s">
         <v>40</v>
       </c>
@@ -4553,7 +4568,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2" t="s">
         <v>379</v>
       </c>
@@ -4571,7 +4586,7 @@
       </c>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2" t="s">
         <v>380</v>
       </c>
@@ -4589,7 +4604,7 @@
       </c>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2" t="s">
         <v>381</v>
       </c>
@@ -4607,7 +4622,7 @@
       </c>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2" t="s">
         <v>382</v>
       </c>
@@ -4625,7 +4640,7 @@
       </c>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="10" t="s">
         <v>94</v>
       </c>
@@ -4650,7 +4665,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
         <v>27</v>
       </c>
@@ -4673,7 +4688,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2" t="s">
         <v>95</v>
       </c>
@@ -4695,7 +4710,7 @@
       </c>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="10" t="s">
         <v>96</v>
       </c>
@@ -4717,7 +4732,7 @@
       </c>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2" t="s">
         <v>383</v>
       </c>
@@ -4734,7 +4749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2" t="s">
         <v>384</v>
       </c>
@@ -4751,7 +4766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2" t="s">
         <v>385</v>
       </c>
@@ -4768,7 +4783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2" t="s">
         <v>386</v>
       </c>
@@ -4785,7 +4800,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2" t="s">
         <v>387</v>
       </c>
@@ -4802,7 +4817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
         <v>97</v>
       </c>
@@ -4825,7 +4840,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="10" t="s">
         <v>46</v>
       </c>
@@ -4846,7 +4861,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2" t="s">
         <v>69</v>
       </c>
@@ -4867,7 +4882,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2" t="s">
         <v>388</v>
       </c>
@@ -4884,7 +4899,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2" t="s">
         <v>33</v>
       </c>
@@ -4907,7 +4922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2" t="s">
         <v>389</v>
       </c>
@@ -4924,7 +4939,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2" t="s">
         <v>390</v>
       </c>
@@ -4941,7 +4956,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2" t="s">
         <v>44</v>
       </c>
@@ -4962,7 +4977,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="10" t="s">
         <v>3</v>
       </c>
@@ -4985,7 +5000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="2" t="s">
         <v>391</v>
       </c>
@@ -5002,7 +5017,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="2" t="s">
         <v>392</v>
       </c>
@@ -5019,7 +5034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2" t="s">
         <v>393</v>
       </c>
@@ -5036,7 +5051,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="2" t="s">
         <v>395</v>
       </c>
@@ -5053,7 +5068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2" t="s">
         <v>8</v>
       </c>
@@ -5076,7 +5091,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2" t="s">
         <v>396</v>
       </c>
@@ -5093,7 +5108,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="2" t="s">
         <v>63</v>
       </c>
@@ -5116,7 +5131,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="10" t="s">
         <v>98</v>
       </c>
@@ -5137,7 +5152,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="10" t="s">
         <v>23</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="2" t="s">
         <v>397</v>
       </c>
@@ -5175,7 +5190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
         <v>60</v>
       </c>
@@ -5198,7 +5213,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="2" t="s">
         <v>68</v>
       </c>
@@ -5219,7 +5234,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="2" t="s">
         <v>398</v>
       </c>
@@ -5236,7 +5251,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="10" t="s">
         <v>54</v>
       </c>
@@ -5257,7 +5272,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="2" t="s">
         <v>399</v>
       </c>
@@ -5274,7 +5289,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="2" t="s">
         <v>400</v>
       </c>
@@ -5291,7 +5306,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="10" t="s">
         <v>100</v>
       </c>
@@ -5312,7 +5327,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="2" t="s">
         <v>402</v>
       </c>
@@ -5329,7 +5344,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="2" t="s">
         <v>403</v>
       </c>
@@ -5346,7 +5361,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="2" t="s">
         <v>404</v>
       </c>
@@ -5363,7 +5378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="2" t="s">
         <v>405</v>
       </c>
@@ -5380,7 +5395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="2" t="s">
         <v>406</v>
       </c>
@@ -5397,7 +5412,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="10" t="s">
         <v>28</v>
       </c>
@@ -5420,7 +5435,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="2" t="s">
         <v>48</v>
       </c>
@@ -5441,7 +5456,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="2" t="s">
         <v>407</v>
       </c>
@@ -5458,7 +5473,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="2" t="s">
         <v>30</v>
       </c>
@@ -5481,7 +5496,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>408</v>
       </c>
@@ -5498,7 +5513,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="10" t="s">
         <v>24</v>
       </c>
@@ -5519,7 +5534,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>409</v>
       </c>
@@ -5536,7 +5551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="2" t="s">
         <v>104</v>
       </c>
@@ -5559,7 +5574,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="2" t="s">
         <v>34</v>
       </c>
@@ -5599,17 +5614,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.41796875" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.68359375" customWidth="1"/>
+    <col min="8" max="10" width="10.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>351</v>
       </c>
@@ -5641,7 +5656,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -5673,7 +5688,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -5712,7 +5727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -5751,7 +5766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -5790,7 +5805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -5829,7 +5844,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
@@ -5868,7 +5883,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>50</v>
       </c>
@@ -5900,7 +5915,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
@@ -5932,7 +5947,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>52</v>
       </c>
@@ -5964,7 +5979,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
@@ -5996,7 +6011,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>75</v>
       </c>
@@ -6028,7 +6043,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>76</v>
       </c>
@@ -6060,7 +6075,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>77</v>
       </c>
@@ -6092,7 +6107,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>78</v>
       </c>
@@ -6124,7 +6139,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>79</v>
       </c>
@@ -6156,7 +6171,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -6188,7 +6203,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>55</v>
       </c>
@@ -6220,7 +6235,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
@@ -6252,7 +6267,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
@@ -6284,7 +6299,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>58</v>
       </c>
@@ -6316,7 +6331,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -6346,7 +6361,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -6378,7 +6393,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -6410,7 +6425,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>11</v>
       </c>
@@ -6442,7 +6457,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -6474,7 +6489,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
@@ -6506,7 +6521,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6" t="s">
         <v>14</v>
       </c>
@@ -6538,7 +6553,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
@@ -6570,7 +6585,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>16</v>
       </c>
@@ -6602,7 +6617,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
@@ -6634,7 +6649,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
@@ -6666,7 +6681,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
@@ -6698,7 +6713,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
@@ -6730,7 +6745,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>21</v>
       </c>
@@ -6762,7 +6777,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>22</v>
       </c>
@@ -6794,7 +6809,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>23</v>
       </c>
@@ -6826,7 +6841,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>24</v>
       </c>
@@ -6858,7 +6873,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>25</v>
       </c>
@@ -6890,7 +6905,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>26</v>
       </c>
@@ -6922,7 +6937,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="6" t="s">
         <v>27</v>
       </c>
@@ -6954,7 +6969,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="14" t="s">
         <v>28</v>
       </c>
@@ -6986,7 +7001,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="14" t="s">
         <v>29</v>
       </c>
@@ -7018,7 +7033,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="14" t="s">
         <v>30</v>
       </c>
@@ -7050,7 +7065,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="14" t="s">
         <v>31</v>
       </c>
@@ -7082,7 +7097,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="14" t="s">
         <v>32</v>
       </c>
@@ -7114,7 +7129,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="14" t="s">
         <v>59</v>
       </c>
@@ -7146,7 +7161,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="14" t="s">
         <v>60</v>
       </c>
@@ -7178,7 +7193,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="14" t="s">
         <v>61</v>
       </c>
@@ -7210,7 +7225,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="14" t="s">
         <v>62</v>
       </c>
@@ -7242,7 +7257,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="14" t="s">
         <v>63</v>
       </c>
@@ -7274,7 +7289,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="14" t="s">
         <v>64</v>
       </c>
@@ -7306,7 +7321,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="14" t="s">
         <v>65</v>
       </c>
@@ -7338,7 +7353,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="14" t="s">
         <v>66</v>
       </c>
@@ -7372,7 +7387,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="14" t="s">
         <v>67</v>
       </c>
@@ -7404,7 +7419,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="14" t="s">
         <v>68</v>
       </c>
@@ -7436,7 +7451,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="14" t="s">
         <v>69</v>
       </c>
@@ -7468,7 +7483,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="14" t="s">
         <v>70</v>
       </c>
@@ -7500,7 +7515,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="14" t="s">
         <v>71</v>
       </c>
@@ -7532,7 +7547,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="14" t="s">
         <v>72</v>
       </c>
@@ -7564,7 +7579,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="14" t="s">
         <v>73</v>
       </c>
@@ -7596,7 +7611,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="14" t="s">
         <v>74</v>
       </c>
@@ -7628,7 +7643,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="14" t="s">
         <v>33</v>
       </c>
@@ -7660,7 +7675,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="14" t="s">
         <v>34</v>
       </c>
@@ -7692,7 +7707,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="14" t="s">
         <v>35</v>
       </c>
@@ -7724,7 +7739,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="14" t="s">
         <v>36</v>
       </c>
@@ -7756,7 +7771,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="14" t="s">
         <v>37</v>
       </c>
@@ -7788,7 +7803,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="14" t="s">
         <v>38</v>
       </c>
@@ -7820,7 +7835,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="14" t="s">
         <v>39</v>
       </c>
@@ -7852,7 +7867,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="14" t="s">
         <v>40</v>
       </c>
@@ -7884,7 +7899,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="14" t="s">
         <v>41</v>
       </c>
@@ -7916,7 +7931,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="14" t="s">
         <v>42</v>
       </c>
@@ -7948,7 +7963,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="14" t="s">
         <v>43</v>
       </c>
@@ -7980,7 +7995,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="14" t="s">
         <v>44</v>
       </c>
@@ -8012,7 +8027,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="14" t="s">
         <v>45</v>
       </c>
@@ -8044,7 +8059,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="14" t="s">
         <v>46</v>
       </c>
@@ -8076,7 +8091,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="14" t="s">
         <v>47</v>
       </c>
@@ -8108,7 +8123,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="14" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
update documentation of search
</commit_message>
<xml_diff>
--- a/02 detailed reviewing results.xlsx
+++ b/02 detailed reviewing results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BE0E2733-190D-4817-B90C-4FE281582992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{622A8877-86CF-40E4-A60D-19D197E08CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviewing Results" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1562" uniqueCount="412">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1561" uniqueCount="412">
   <si>
     <t>Title</t>
   </si>
@@ -2199,26 +2199,26 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.26171875" customWidth="1"/>
-    <col min="2" max="2" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.15625" customWidth="1"/>
-    <col min="4" max="4" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.68359375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.26171875" customWidth="1"/>
+    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>83</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>37</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>49</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>78</v>
       </c>
@@ -2469,8 +2469,11 @@
       <c r="J9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
@@ -2524,7 +2527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>88</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>66</v>
       </c>
@@ -2672,11 +2675,8 @@
       <c r="J17">
         <v>16</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>75</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>79</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>72</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>11</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>1</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>22</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>52</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>45</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>99</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>64</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>101</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>17</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>57</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>7</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>62</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>103</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>50</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>71</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>70</v>
       </c>
@@ -3513,11 +3513,8 @@
       <c r="J49">
         <v>48</v>
       </c>
-      <c r="K49" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>39</v>
       </c>
@@ -3543,7 +3540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>12</v>
       </c>
@@ -3566,7 +3563,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>82</v>
       </c>
@@ -3589,7 +3586,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -3609,7 +3606,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -3629,7 +3626,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>355</v>
       </c>
@@ -3651,7 +3648,7 @@
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
@@ -3671,7 +3668,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>356</v>
       </c>
@@ -3693,7 +3690,7 @@
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>357</v>
       </c>
@@ -3715,7 +3712,7 @@
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
@@ -3737,7 +3734,7 @@
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>359</v>
       </c>
@@ -3759,7 +3756,7 @@
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>361</v>
       </c>
@@ -3781,7 +3778,7 @@
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>84</v>
       </c>
@@ -3804,7 +3801,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>47</v>
       </c>
@@ -3821,7 +3818,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -3838,7 +3835,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>362</v>
       </c>
@@ -3860,7 +3857,7 @@
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>364</v>
       </c>
@@ -3882,7 +3879,7 @@
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>59</v>
       </c>
@@ -3906,7 +3903,7 @@
       </c>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>365</v>
       </c>
@@ -3928,7 +3925,7 @@
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>85</v>
       </c>
@@ -3947,7 +3944,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>42</v>
       </c>
@@ -3964,7 +3961,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>366</v>
       </c>
@@ -3986,7 +3983,7 @@
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>43</v>
       </c>
@@ -4003,7 +4000,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>367</v>
       </c>
@@ -4025,7 +4022,7 @@
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>86</v>
       </c>
@@ -4048,7 +4045,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>368</v>
       </c>
@@ -4070,7 +4067,7 @@
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>25</v>
       </c>
@@ -4091,7 +4088,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>76</v>
       </c>
@@ -4112,7 +4109,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>369</v>
       </c>
@@ -4134,7 +4131,7 @@
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>87</v>
       </c>
@@ -4159,7 +4156,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>370</v>
       </c>
@@ -4177,7 +4174,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>371</v>
       </c>
@@ -4195,7 +4192,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>77</v>
       </c>
@@ -4218,7 +4215,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>32</v>
       </c>
@@ -4243,7 +4240,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>89</v>
       </c>
@@ -4268,7 +4265,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>90</v>
       </c>
@@ -4293,7 +4290,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>35</v>
       </c>
@@ -4316,7 +4313,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>372</v>
       </c>
@@ -4334,7 +4331,7 @@
       </c>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>92</v>
       </c>
@@ -4359,7 +4356,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>373</v>
       </c>
@@ -4377,7 +4374,7 @@
       </c>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>93</v>
       </c>
@@ -4400,7 +4397,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>14</v>
       </c>
@@ -4425,7 +4422,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>58</v>
       </c>
@@ -4448,7 +4445,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>375</v>
       </c>
@@ -4466,7 +4463,7 @@
       </c>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>376</v>
       </c>
@@ -4484,7 +4481,7 @@
       </c>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>377</v>
       </c>
@@ -4502,7 +4499,7 @@
       </c>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>378</v>
       </c>
@@ -4520,7 +4517,7 @@
       </c>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>31</v>
       </c>
@@ -4545,7 +4542,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>40</v>
       </c>
@@ -4568,7 +4565,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>379</v>
       </c>
@@ -4586,7 +4583,7 @@
       </c>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>380</v>
       </c>
@@ -4604,7 +4601,7 @@
       </c>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>381</v>
       </c>
@@ -4622,7 +4619,7 @@
       </c>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>382</v>
       </c>
@@ -4640,7 +4637,7 @@
       </c>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>94</v>
       </c>
@@ -4665,7 +4662,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
         <v>27</v>
       </c>
@@ -4688,7 +4685,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>95</v>
       </c>
@@ -4710,7 +4707,7 @@
       </c>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
         <v>96</v>
       </c>
@@ -4732,7 +4729,7 @@
       </c>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>383</v>
       </c>
@@ -4749,7 +4746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>384</v>
       </c>
@@ -4766,7 +4763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>385</v>
       </c>
@@ -4783,7 +4780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>386</v>
       </c>
@@ -4800,7 +4797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>387</v>
       </c>
@@ -4817,7 +4814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>97</v>
       </c>
@@ -4840,7 +4837,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>46</v>
       </c>
@@ -4861,7 +4858,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>69</v>
       </c>
@@ -4882,7 +4879,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>388</v>
       </c>
@@ -4899,7 +4896,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>33</v>
       </c>
@@ -4922,7 +4919,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>389</v>
       </c>
@@ -4939,7 +4936,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>390</v>
       </c>
@@ -4956,7 +4953,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>44</v>
       </c>
@@ -4977,7 +4974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
         <v>3</v>
       </c>
@@ -5000,7 +4997,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>391</v>
       </c>
@@ -5017,7 +5014,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>392</v>
       </c>
@@ -5034,7 +5031,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>393</v>
       </c>
@@ -5051,7 +5048,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>395</v>
       </c>
@@ -5068,7 +5065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>8</v>
       </c>
@@ -5091,7 +5088,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>396</v>
       </c>
@@ -5108,7 +5105,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>63</v>
       </c>
@@ -5131,7 +5128,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>98</v>
       </c>
@@ -5152,7 +5149,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>23</v>
       </c>
@@ -5173,7 +5170,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>397</v>
       </c>
@@ -5190,7 +5187,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>60</v>
       </c>
@@ -5213,7 +5210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>68</v>
       </c>
@@ -5234,7 +5231,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>398</v>
       </c>
@@ -5251,7 +5248,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>54</v>
       </c>
@@ -5272,7 +5269,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>399</v>
       </c>
@@ -5289,7 +5286,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>400</v>
       </c>
@@ -5306,7 +5303,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>100</v>
       </c>
@@ -5327,7 +5324,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>402</v>
       </c>
@@ -5344,7 +5341,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>403</v>
       </c>
@@ -5361,7 +5358,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>404</v>
       </c>
@@ -5378,7 +5375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>405</v>
       </c>
@@ -5395,7 +5392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>406</v>
       </c>
@@ -5412,7 +5409,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>28</v>
       </c>
@@ -5435,7 +5432,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>48</v>
       </c>
@@ -5456,7 +5453,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>407</v>
       </c>
@@ -5473,7 +5470,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>30</v>
       </c>
@@ -5496,7 +5493,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>408</v>
       </c>
@@ -5513,7 +5510,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="s">
         <v>24</v>
       </c>
@@ -5534,7 +5531,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>409</v>
       </c>
@@ -5551,7 +5548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>104</v>
       </c>
@@ -5574,7 +5571,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>34</v>
       </c>
@@ -5614,17 +5611,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26171875" customWidth="1"/>
-    <col min="3" max="3" width="17.41796875" customWidth="1"/>
-    <col min="5" max="5" width="14.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.68359375" customWidth="1"/>
-    <col min="8" max="10" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>351</v>
       </c>
@@ -5656,7 +5653,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -5688,7 +5685,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -5727,7 +5724,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -5766,7 +5763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -5805,7 +5802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -5844,7 +5841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
@@ -5883,7 +5880,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>50</v>
       </c>
@@ -5915,7 +5912,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
@@ -5947,7 +5944,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>52</v>
       </c>
@@ -5979,7 +5976,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
@@ -6011,7 +6008,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>75</v>
       </c>
@@ -6043,7 +6040,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>76</v>
       </c>
@@ -6075,7 +6072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>77</v>
       </c>
@@ -6107,7 +6104,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>78</v>
       </c>
@@ -6139,7 +6136,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>79</v>
       </c>
@@ -6171,7 +6168,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -6203,7 +6200,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>55</v>
       </c>
@@ -6235,7 +6232,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
@@ -6267,7 +6264,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
@@ -6299,7 +6296,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>58</v>
       </c>
@@ -6331,7 +6328,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -6361,7 +6358,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -6393,7 +6390,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -6425,7 +6422,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>11</v>
       </c>
@@ -6457,7 +6454,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -6489,7 +6486,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
@@ -6521,7 +6518,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>14</v>
       </c>
@@ -6553,7 +6550,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
@@ -6585,7 +6582,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>16</v>
       </c>
@@ -6617,7 +6614,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
@@ -6649,7 +6646,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
@@ -6681,7 +6678,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
@@ -6713,7 +6710,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
@@ -6745,7 +6742,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>21</v>
       </c>
@@ -6777,7 +6774,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>22</v>
       </c>
@@ -6809,7 +6806,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>23</v>
       </c>
@@ -6841,7 +6838,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>24</v>
       </c>
@@ -6873,7 +6870,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>25</v>
       </c>
@@ -6905,7 +6902,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>26</v>
       </c>
@@ -6937,7 +6934,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>27</v>
       </c>
@@ -6969,7 +6966,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>28</v>
       </c>
@@ -7001,7 +6998,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>29</v>
       </c>
@@ -7033,7 +7030,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>30</v>
       </c>
@@ -7065,7 +7062,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>31</v>
       </c>
@@ -7097,7 +7094,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>32</v>
       </c>
@@ -7129,7 +7126,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>59</v>
       </c>
@@ -7161,7 +7158,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>60</v>
       </c>
@@ -7193,7 +7190,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>61</v>
       </c>
@@ -7225,7 +7222,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>62</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>63</v>
       </c>
@@ -7289,7 +7286,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>64</v>
       </c>
@@ -7321,7 +7318,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>65</v>
       </c>
@@ -7353,7 +7350,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>66</v>
       </c>
@@ -7387,7 +7384,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>67</v>
       </c>
@@ -7419,7 +7416,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>68</v>
       </c>
@@ -7451,7 +7448,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>69</v>
       </c>
@@ -7483,7 +7480,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>70</v>
       </c>
@@ -7515,7 +7512,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>71</v>
       </c>
@@ -7547,7 +7544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>72</v>
       </c>
@@ -7579,7 +7576,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>73</v>
       </c>
@@ -7611,7 +7608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>74</v>
       </c>
@@ -7643,7 +7640,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>33</v>
       </c>
@@ -7675,7 +7672,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>34</v>
       </c>
@@ -7707,7 +7704,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>35</v>
       </c>
@@ -7739,7 +7736,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>36</v>
       </c>
@@ -7771,7 +7768,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>37</v>
       </c>
@@ -7803,7 +7800,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>38</v>
       </c>
@@ -7835,7 +7832,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>39</v>
       </c>
@@ -7867,7 +7864,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>40</v>
       </c>
@@ -7899,7 +7896,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>41</v>
       </c>
@@ -7931,7 +7928,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>42</v>
       </c>
@@ -7963,7 +7960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>43</v>
       </c>
@@ -7995,7 +7992,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>44</v>
       </c>
@@ -8027,7 +8024,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>45</v>
       </c>
@@ -8059,7 +8056,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>46</v>
       </c>
@@ -8091,7 +8088,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>47</v>
       </c>
@@ -8123,7 +8120,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>48</v>
       </c>

</xml_diff>